<commit_message>
feat: query newly added question to game
</commit_message>
<xml_diff>
--- a/test/Game 4 Good - Questions Input - Spanish.xlsx
+++ b/test/Game 4 Good - Questions Input - Spanish.xlsx
@@ -37,10 +37,10 @@
     <t>answer</t>
   </si>
   <si>
-    <t>match</t>
-  </si>
-  <si>
-    <t>spanish</t>
+    <t>Matching</t>
+  </si>
+  <si>
+    <t>Spanish</t>
   </si>
   <si>
     <t>Resolución</t>

</xml_diff>